<commit_message>
Funcao que calcula o melhor valor de K para cada liga
</commit_message>
<xml_diff>
--- a/Previsao_de_jogos_lol/TIMES.xlsx
+++ b/Previsao_de_jogos_lol/TIMES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac02/Desktop/Previsão League of Legends/TESTE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac02/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70F9CFC-A785-5643-85FD-B96203CD1051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F115C84B-F679-6940-BE5F-A62735659DAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31940" yWindow="3700" windowWidth="13680" windowHeight="23480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Times" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,6 +498,13 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Aparajita"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -696,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -731,6 +738,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1013,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1050,7 +1058,7 @@
       <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -1069,8 +1077,8 @@
       <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>35</v>
+      <c r="B3" s="26" t="s">
+        <v>37</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>44</v>
@@ -1088,8 +1096,8 @@
       <c r="A4" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>36</v>
+      <c r="B4" s="26" t="s">
+        <v>136</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>44</v>
@@ -1105,8 +1113,8 @@
       <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>37</v>
+      <c r="B5" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>44</v>
@@ -1122,8 +1130,8 @@
       <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>136</v>
+      <c r="B6" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>44</v>
@@ -1139,7 +1147,7 @@
       <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -1156,7 +1164,7 @@
       <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="18" t="s">
@@ -1173,7 +1181,7 @@
       <c r="A9" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="18" t="s">
@@ -1190,7 +1198,7 @@
       <c r="A10" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -1207,7 +1215,7 @@
       <c r="A11" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -1225,7 +1233,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>90</v>
@@ -1242,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>90</v>
@@ -1259,7 +1267,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>90</v>
@@ -1310,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>90</v>
@@ -1344,7 +1352,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>90</v>
@@ -1361,7 +1369,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>90</v>
@@ -1378,7 +1386,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>90</v>
@@ -1395,7 +1403,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>90</v>
@@ -1412,7 +1420,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>90</v>
@@ -1429,7 +1437,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>90</v>
@@ -1497,7 +1505,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>134</v>
@@ -1531,7 +1539,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>134</v>
@@ -1633,7 +1641,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>33</v>
@@ -1650,7 +1658,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>33</v>
@@ -1820,7 +1828,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>98</v>
@@ -1837,7 +1845,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>98</v>

</xml_diff>